<commit_message>
feat: add updating pricing data file
</commit_message>
<xml_diff>
--- a/output/cost_report.xlsx
+++ b/output/cost_report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>$15.00</t>
+          <t>$20.00</t>
         </is>
       </c>
     </row>
@@ -476,15 +476,27 @@
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ALB</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>$18.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Total Estimated Monthly Cost</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>$28.02</t>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>$51.02</t>
         </is>
       </c>
     </row>

</xml_diff>